<commit_message>
Api thu so v2, cap nhat gia ban
</commit_message>
<xml_diff>
--- a/src/assets/upload-product.xlsx
+++ b/src/assets/upload-product.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\G99-Product\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\G99_PROJECTS_FRONTNED\admin.s198\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018C4A1F-6582-47F4-87E7-2BDAD28D1A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018E1DF1-0065-45F4-A2EA-C94118013E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>NAME</t>
   </si>
@@ -31,9 +31,6 @@
     <t>DESC</t>
   </si>
   <si>
-    <t>hello</t>
-  </si>
-  <si>
     <t>SKU</t>
   </si>
   <si>
@@ -46,13 +43,13 @@
     <t>BRAND</t>
   </si>
   <si>
-    <t>VTT</t>
-  </si>
-  <si>
     <t>STOCK_QUANTITY</t>
   </si>
   <si>
-    <t>0999999997</t>
+    <t>0993000001</t>
+  </si>
+  <si>
+    <t>VNP</t>
   </si>
 </sst>
 </file>
@@ -71,6 +68,7 @@
       <b/>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -434,7 +432,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,41 +452,38 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>50000</v>
+      </c>
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>999999997</v>
-      </c>
-      <c r="E2">
-        <v>600000</v>
-      </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>1</v>

</xml_diff>

<commit_message>
upload nhieu file, kitting
</commit_message>
<xml_diff>
--- a/src/assets/upload-product.xlsx
+++ b/src/assets/upload-product.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\G99_PROJECTS_FRONTNED\admin.s198\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018E1DF1-0065-45F4-A2EA-C94118013E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF270B2-A09D-4946-B933-32A7C2A3786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="Hướng dẫn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>NAME</t>
   </si>
@@ -50,13 +51,88 @@
   </si>
   <si>
     <t>VNP</t>
+  </si>
+  <si>
+    <t>- SHORT_DESC: Mô tả ngắn (Có thể điền hoặc không điền). </t>
+  </si>
+  <si>
+    <t>- DESC: Mô tả (Có thể điền hoặc không điền).</t>
+  </si>
+  <si>
+    <t>- SKU: Mã số (Bắt buộc phải điền).</t>
+  </si>
+  <si>
+    <t>Điền giống như NAME.</t>
+  </si>
+  <si>
+    <t>- PRICE: Giá cả (Có thể điền hoặc không điền).</t>
+  </si>
+  <si>
+    <t>Điền</t>
+  </si>
+  <si>
+    <t>VMS - MOBIPHONE.</t>
+  </si>
+  <si>
+    <t>VNM - VIETNAMOBILE.</t>
+  </si>
+  <si>
+    <t>VNP - VINAPHONE.</t>
+  </si>
+  <si>
+    <t>GSIM.</t>
+  </si>
+  <si>
+    <t>VTT - VIETTEL.</t>
+  </si>
+  <si>
+    <t>- STOCK_QUANTITY: Số lượng (Có thể điền hoặc không điền).</t>
+  </si>
+  <si>
+    <t>- LEVEL: Hạng số. (Có thể điền hoặc không điền).</t>
+  </si>
+  <si>
+    <t>NORMAL.</t>
+  </si>
+  <si>
+    <t>QUASI.</t>
+  </si>
+  <si>
+    <t>BRONZE.</t>
+  </si>
+  <si>
+    <t>SILVER.</t>
+  </si>
+  <si>
+    <t>GOLD.</t>
+  </si>
+  <si>
+    <t>PLATINUM</t>
+  </si>
+  <si>
+    <t>- NAME: Số điện thoại/Số serial (Bắt buộc phải điền).</t>
+  </si>
+  <si>
+    <t>- CATEGORY_ID: Loại sản phẩm (Bắt buộc điền).</t>
+  </si>
+  <si>
+    <t>3 là số điện thoại</t>
+  </si>
+  <si>
+    <t>2 là serial SIM</t>
+  </si>
+  <si>
+    <t>- BRAND: Tên nhà mạng (Bắt buộc điền).</t>
+  </si>
+  <si>
+    <t>LEVEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -67,6 +143,32 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -106,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -115,6 +217,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +548,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +582,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -492,4 +610,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B659D42-4769-423E-A3A5-32E257AB1352}">
+  <dimension ref="B2:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="5.140625" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C20" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C24" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C26" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>